<commit_message>
Actualización del cuaderno de predicción, incluyendo modelos LSTM, Markov, Poisson y Binomial Negativa. Se añadieron datos en tombola.xlsx.
</commit_message>
<xml_diff>
--- a/data/tombola.xlsx
+++ b/data/tombola.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bec0d9ad08ccde7/Programacion/6 - Otros/TombolaMisionera/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bec0d9ad08ccde7/Programacion/6 - Otros/Prediccion-Bingo-Municipal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_243EA73E763B8A2E925890EC474C1A594E8B07D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6264D33-EB22-409C-8D51-7858D8AC8E3C}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="11_243EA73E763B8A2E925890EC474C1A594E8B07D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B75F2E94-2148-4D85-AA04-9E94D0656DA6}"/>
   <bookViews>
-    <workbookView xWindow="24810" yWindow="4110" windowWidth="18780" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20055" yWindow="3585" windowWidth="18780" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -73,10 +73,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -295,10 +295,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -306,7 +306,7 @@
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -317,7 +317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45859</v>
       </c>
@@ -328,7 +328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45859</v>
       </c>
@@ -339,7 +339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45859</v>
       </c>
@@ -350,7 +350,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45859</v>
       </c>
@@ -361,7 +361,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45859</v>
       </c>
@@ -372,7 +372,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45859</v>
       </c>
@@ -383,7 +383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45859</v>
       </c>
@@ -394,7 +394,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45859</v>
       </c>
@@ -405,7 +405,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45859</v>
       </c>
@@ -416,7 +416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45859</v>
       </c>
@@ -427,7 +427,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45860</v>
       </c>
@@ -438,7 +438,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45860</v>
       </c>
@@ -449,7 +449,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45860</v>
       </c>
@@ -460,7 +460,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45860</v>
       </c>
@@ -471,7 +471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45860</v>
       </c>
@@ -482,7 +482,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45860</v>
       </c>
@@ -493,7 +493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45860</v>
       </c>
@@ -504,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>45860</v>
       </c>
@@ -515,7 +515,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>45860</v>
       </c>
@@ -526,7 +526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>45860</v>
       </c>
@@ -537,7 +537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>45861</v>
       </c>
@@ -548,7 +548,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>45861</v>
       </c>
@@ -559,7 +559,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>45861</v>
       </c>
@@ -570,7 +570,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>45861</v>
       </c>
@@ -581,7 +581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>45861</v>
       </c>
@@ -592,7 +592,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>45861</v>
       </c>
@@ -603,7 +603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>45861</v>
       </c>
@@ -614,7 +614,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>45861</v>
       </c>
@@ -625,7 +625,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>45861</v>
       </c>
@@ -636,7 +636,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45861</v>
       </c>
@@ -647,7 +647,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45862</v>
       </c>
@@ -658,7 +658,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45862</v>
       </c>
@@ -669,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45862</v>
       </c>
@@ -680,7 +680,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>45862</v>
       </c>
@@ -691,7 +691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45862</v>
       </c>
@@ -702,7 +702,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45862</v>
       </c>
@@ -713,7 +713,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45862</v>
       </c>
@@ -724,7 +724,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45862</v>
       </c>
@@ -735,7 +735,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45862</v>
       </c>
@@ -746,7 +746,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45862</v>
       </c>
@@ -757,7 +757,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45863</v>
       </c>
@@ -768,7 +768,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45863</v>
       </c>
@@ -779,7 +779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45863</v>
       </c>
@@ -790,7 +790,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45863</v>
       </c>
@@ -801,7 +801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45863</v>
       </c>
@@ -812,7 +812,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>45863</v>
       </c>
@@ -823,7 +823,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45863</v>
       </c>
@@ -834,7 +834,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>45863</v>
       </c>
@@ -845,7 +845,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>45863</v>
       </c>
@@ -856,7 +856,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>45863</v>
       </c>
@@ -867,7 +867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>45864</v>
       </c>
@@ -878,7 +878,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>45864</v>
       </c>
@@ -889,7 +889,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>45864</v>
       </c>
@@ -900,7 +900,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>45864</v>
       </c>
@@ -911,7 +911,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>45864</v>
       </c>
@@ -922,7 +922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>45864</v>
       </c>
@@ -933,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>45864</v>
       </c>
@@ -944,7 +944,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>45864</v>
       </c>
@@ -955,7 +955,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>45864</v>
       </c>
@@ -966,7 +966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>45864</v>
       </c>
@@ -977,7 +977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>45852</v>
       </c>
@@ -988,7 +988,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>45852</v>
       </c>
@@ -999,7 +999,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>45852</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>45852</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>45852</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>45852</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>45852</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>45852</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>45852</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>45852</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>45853</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>45853</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>45853</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>45853</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>45853</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>45853</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>45853</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>45853</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>45853</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>45853</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>45854</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>45854</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>45854</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>45854</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>45854</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>45854</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>45854</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>45854</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>45854</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>45854</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>45855</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>45855</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>45855</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>45855</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>45855</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>45855</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>45855</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>45855</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>45855</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>45855</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>45856</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>45856</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>45856</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>45856</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>45856</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>45856</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>45856</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>45856</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>45856</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>45856</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>45857</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>45857</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>45857</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>45857</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>45857</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>45857</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>45857</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>45857</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>45857</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>45857</v>
       </c>
@@ -1745,6 +1745,556 @@
       </c>
       <c r="C131" s="1">
         <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B132" s="1">
+        <v>1</v>
+      </c>
+      <c r="C132" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B133" s="1">
+        <v>2</v>
+      </c>
+      <c r="C133" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B134" s="1">
+        <v>3</v>
+      </c>
+      <c r="C134" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B135" s="1">
+        <v>4</v>
+      </c>
+      <c r="C135" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B136" s="1">
+        <v>5</v>
+      </c>
+      <c r="C136" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B137" s="1">
+        <v>6</v>
+      </c>
+      <c r="C137" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B138" s="1">
+        <v>7</v>
+      </c>
+      <c r="C138" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B139" s="1">
+        <v>8</v>
+      </c>
+      <c r="C139" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B140" s="1">
+        <v>9</v>
+      </c>
+      <c r="C140" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="3">
+        <v>45867</v>
+      </c>
+      <c r="B141" s="1">
+        <v>10</v>
+      </c>
+      <c r="C141" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B142" s="1">
+        <v>1</v>
+      </c>
+      <c r="C142" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B143" s="1">
+        <v>2</v>
+      </c>
+      <c r="C143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B144" s="1">
+        <v>3</v>
+      </c>
+      <c r="C144" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B145" s="1">
+        <v>4</v>
+      </c>
+      <c r="C145" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B146" s="1">
+        <v>5</v>
+      </c>
+      <c r="C146" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B147" s="1">
+        <v>6</v>
+      </c>
+      <c r="C147" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B148" s="1">
+        <v>7</v>
+      </c>
+      <c r="C148" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B149" s="1">
+        <v>8</v>
+      </c>
+      <c r="C149" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B150" s="1">
+        <v>9</v>
+      </c>
+      <c r="C150" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B151" s="1">
+        <v>10</v>
+      </c>
+      <c r="C151" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B152" s="1">
+        <v>1</v>
+      </c>
+      <c r="C152" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B153" s="1">
+        <v>2</v>
+      </c>
+      <c r="C153" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B154" s="1">
+        <v>3</v>
+      </c>
+      <c r="C154" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B155" s="1">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B156" s="1">
+        <v>5</v>
+      </c>
+      <c r="C156" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B157" s="1">
+        <v>6</v>
+      </c>
+      <c r="C157" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B158" s="1">
+        <v>7</v>
+      </c>
+      <c r="C158" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B159" s="1">
+        <v>8</v>
+      </c>
+      <c r="C159" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B160" s="1">
+        <v>9</v>
+      </c>
+      <c r="C160" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
+        <v>45869</v>
+      </c>
+      <c r="B161" s="1">
+        <v>10</v>
+      </c>
+      <c r="C161" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B162" s="1">
+        <v>1</v>
+      </c>
+      <c r="C162" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B163" s="1">
+        <v>2</v>
+      </c>
+      <c r="C163" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B164" s="1">
+        <v>3</v>
+      </c>
+      <c r="C164" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B165" s="1">
+        <v>4</v>
+      </c>
+      <c r="C165" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B166" s="1">
+        <v>5</v>
+      </c>
+      <c r="C166" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B167" s="1">
+        <v>6</v>
+      </c>
+      <c r="C167" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B168" s="1">
+        <v>7</v>
+      </c>
+      <c r="C168" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B169" s="1">
+        <v>8</v>
+      </c>
+      <c r="C169" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B170" s="1">
+        <v>9</v>
+      </c>
+      <c r="C170" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="3">
+        <v>45870</v>
+      </c>
+      <c r="B171" s="1">
+        <v>10</v>
+      </c>
+      <c r="C171" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B172" s="1">
+        <v>1</v>
+      </c>
+      <c r="C172" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B173" s="1">
+        <v>2</v>
+      </c>
+      <c r="C173" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B174" s="1">
+        <v>3</v>
+      </c>
+      <c r="C174" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B175" s="1">
+        <v>4</v>
+      </c>
+      <c r="C175" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B176" s="1">
+        <v>5</v>
+      </c>
+      <c r="C176" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B177" s="1">
+        <v>6</v>
+      </c>
+      <c r="C177" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B178" s="1">
+        <v>7</v>
+      </c>
+      <c r="C178" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B179" s="1">
+        <v>8</v>
+      </c>
+      <c r="C179" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B180" s="1">
+        <v>9</v>
+      </c>
+      <c r="C180" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="3">
+        <v>45871</v>
+      </c>
+      <c r="B181" s="1">
+        <v>10</v>
+      </c>
+      <c r="C181" s="1">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrige los recuentos de ejecución del modelo de predicción y los mensajes de salida.
Restablece los recuentos de ejecución en el cuaderno de Jupyter para mantener la coherencia y actualiza los mensajes de salida para reflejar el número correcto de predicciones generadas.

Refina la gestión de datos en el script del modelo LSTM filtrando secuencias según fechas y garantizando una agrupación adecuada de datos para las predicciones.

Mejora la legibilidad y mantiene la funcionalidad eliminando comentarios innecesarios y garantizando rutas precisas para los modelos guardados y los archivos CSV.
</commit_message>
<xml_diff>
--- a/data/tombola.xlsx
+++ b/data/tombola.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bec0d9ad08ccde7/Programacion/6 - Otros/Prediccion-Bingo-Municipal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_243EA73E763B8A2E925890EC474C1A594E8B07D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B75F2E94-2148-4D85-AA04-9E94D0656DA6}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="11_243EA73E763B8A2E925890EC474C1A594E8B07D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9BA65F2-5609-4B01-BE8A-95B522B26520}"/>
   <bookViews>
     <workbookView xWindow="20055" yWindow="3585" windowWidth="18780" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,6 +92,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -295,10 +299,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2297,6 +2301,446 @@
         <v>9</v>
       </c>
     </row>
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B182" s="1">
+        <v>1</v>
+      </c>
+      <c r="C182" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B183" s="1">
+        <v>2</v>
+      </c>
+      <c r="C183" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B184" s="1">
+        <v>3</v>
+      </c>
+      <c r="C184" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B185" s="1">
+        <v>4</v>
+      </c>
+      <c r="C185" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B186" s="1">
+        <v>5</v>
+      </c>
+      <c r="C186" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B187" s="1">
+        <v>6</v>
+      </c>
+      <c r="C187" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B188" s="1">
+        <v>7</v>
+      </c>
+      <c r="C188" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B189" s="1">
+        <v>8</v>
+      </c>
+      <c r="C189" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B190" s="1">
+        <v>9</v>
+      </c>
+      <c r="C190" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B191" s="1">
+        <v>10</v>
+      </c>
+      <c r="C191" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B192" s="1">
+        <v>1</v>
+      </c>
+      <c r="C192" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B193" s="1">
+        <v>2</v>
+      </c>
+      <c r="C193" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B194" s="1">
+        <v>3</v>
+      </c>
+      <c r="C194" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B195" s="1">
+        <v>4</v>
+      </c>
+      <c r="C195" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B196" s="1">
+        <v>5</v>
+      </c>
+      <c r="C196" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B197" s="1">
+        <v>6</v>
+      </c>
+      <c r="C197" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B198" s="1">
+        <v>7</v>
+      </c>
+      <c r="C198" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B199" s="1">
+        <v>8</v>
+      </c>
+      <c r="C199" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B200" s="1">
+        <v>9</v>
+      </c>
+      <c r="C200" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B201" s="1">
+        <v>10</v>
+      </c>
+      <c r="C201" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B202" s="1">
+        <v>1</v>
+      </c>
+      <c r="C202" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B203" s="1">
+        <v>2</v>
+      </c>
+      <c r="C203" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B204" s="1">
+        <v>3</v>
+      </c>
+      <c r="C204" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B205" s="1">
+        <v>4</v>
+      </c>
+      <c r="C205" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B206" s="1">
+        <v>5</v>
+      </c>
+      <c r="C206" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B207" s="1">
+        <v>6</v>
+      </c>
+      <c r="C207" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B208" s="1">
+        <v>7</v>
+      </c>
+      <c r="C208" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B209" s="1">
+        <v>8</v>
+      </c>
+      <c r="C209" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B210" s="1">
+        <v>9</v>
+      </c>
+      <c r="C210" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B211" s="1">
+        <v>10</v>
+      </c>
+      <c r="C211" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B212" s="1">
+        <v>1</v>
+      </c>
+      <c r="C212" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B213" s="1">
+        <v>2</v>
+      </c>
+      <c r="C213" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B214" s="1">
+        <v>3</v>
+      </c>
+      <c r="C214" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B215" s="1">
+        <v>4</v>
+      </c>
+      <c r="C215" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B216" s="1">
+        <v>5</v>
+      </c>
+      <c r="C216" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B217" s="1">
+        <v>6</v>
+      </c>
+      <c r="C217" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B218" s="1">
+        <v>7</v>
+      </c>
+      <c r="C218" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B219" s="1">
+        <v>8</v>
+      </c>
+      <c r="C219" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B220" s="1">
+        <v>9</v>
+      </c>
+      <c r="C220" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B221" s="1">
+        <v>10</v>
+      </c>
+      <c r="C221" s="1">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>